<commit_message>
Editar eliminar, productos, boxes
</commit_message>
<xml_diff>
--- a/modelo BDD/plantilla importacion Productos.xlsx
+++ b/modelo BDD/plantilla importacion Productos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ItemsType" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,10 @@
     <sheet name="PROCESS" sheetId="3" r:id="rId3"/>
     <sheet name="SPECIES" sheetId="8" r:id="rId4"/>
     <sheet name="Variety" sheetId="4" r:id="rId5"/>
-    <sheet name="Color" sheetId="5" r:id="rId6"/>
-    <sheet name="Grade" sheetId="6" r:id="rId7"/>
-    <sheet name="Cuts" sheetId="7" r:id="rId8"/>
+    <sheet name="typeBoxe" sheetId="9" r:id="rId6"/>
+    <sheet name="Color" sheetId="5" r:id="rId7"/>
+    <sheet name="Grade" sheetId="6" r:id="rId8"/>
+    <sheet name="Cuts" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="373">
   <si>
     <t>TYPE</t>
   </si>
@@ -1132,13 +1133,31 @@
   </si>
   <si>
     <t>PINK O HARA</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>PG</t>
+  </si>
+  <si>
+    <t>QB</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>EB</t>
+  </si>
+  <si>
+    <t>HB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1188,6 +1207,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1239,7 +1264,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1289,6 +1314,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2291,7 +2319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F229"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1:F229"/>
     </sheetView>
   </sheetViews>
@@ -8019,6 +8047,76 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="B1" t="str">
+        <f t="shared" ref="B1:B6" si="0">CONCATENATE("insert into(TYPEBOXE_BTYPE,DATECREATE_BTYPE) values('",A1,"',getdate() ),")</f>
+        <v>insert into(TYPEBOXE_BTYPE,DATECREATE_BTYPE) values('SB',getdate() ),</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>368</v>
+      </c>
+      <c r="B2" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into(TYPEBOXE_BTYPE,DATECREATE_BTYPE) values('PG',getdate() ),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into(TYPEBOXE_BTYPE,DATECREATE_BTYPE) values('QB',getdate() ),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into(TYPEBOXE_BTYPE,DATECREATE_BTYPE) values('Vendor',getdate() ),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into(TYPEBOXE_BTYPE,DATECREATE_BTYPE) values('EB',getdate() ),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into(TYPEBOXE_BTYPE,DATECREATE_BTYPE) values('HB',getdate() ),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C137"/>
   <sheetViews>
@@ -9813,7 +9911,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B35"/>
   <sheetViews>
@@ -10146,7 +10244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>

</xml_diff>